<commit_message>
imports excel file safe
</commit_message>
<xml_diff>
--- a/database/spreadsheet/test/Test File 1.xlsx
+++ b/database/spreadsheet/test/Test File 1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GOVCONSERVER\RedirectedFolders\snudel\Desktop\Test Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\GSA-Advantage-Scraper\database\spreadsheet\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="285">
   <si>
     <t>SIN</t>
   </si>
@@ -870,13 +870,22 @@
   </si>
   <si>
     <t>Lined Duty Belt  Lined Duty Belt58 Hi-Gloss Finish Fits 58 in. waist (147cm)</t>
+  </si>
+  <si>
+    <t>MONADNOCK</t>
+  </si>
+  <si>
+    <t>GOULD</t>
+  </si>
+  <si>
+    <t>GOODRICH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -935,7 +944,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -948,12 +957,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -983,7 +1015,12 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1291,16 +1328,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="6" max="6" width="74.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1323,7 +1367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1346,7 +1390,7 @@
         <v>22.458400000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1369,12 +1413,12 @@
         <v>22.458400000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
+      <c r="B4" s="6" t="s">
+        <v>282</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>15</v>
@@ -1392,11 +1436,11 @@
         <v>24.623840000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1415,7 +1459,7 @@
         <v>22.458400000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1438,7 +1482,7 @@
         <v>156.31904</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1461,7 +1505,7 @@
         <v>156.31904</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1484,7 +1528,7 @@
         <v>156.31904</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1507,7 +1551,7 @@
         <v>103.94112</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1530,7 +1574,7 @@
         <v>162.13999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1553,7 +1597,7 @@
         <v>39.840000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1576,7 +1620,7 @@
         <v>39.840000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1599,7 +1643,7 @@
         <v>26.79</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -1622,7 +1666,7 @@
         <v>26.79</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1645,7 +1689,7 @@
         <v>32.590000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1668,7 +1712,7 @@
         <v>39.81</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1691,7 +1735,7 @@
         <v>32.590000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1714,7 +1758,7 @@
         <v>26.79</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1737,7 +1781,7 @@
         <v>39.840000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1760,7 +1804,7 @@
         <v>39.840000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -1783,7 +1827,7 @@
         <v>33.99</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1806,7 +1850,7 @@
         <v>33.99</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -1829,7 +1873,7 @@
         <v>33.99</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1852,7 +1896,7 @@
         <v>52.12</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -1875,7 +1919,7 @@
         <v>52.12</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -1898,7 +1942,7 @@
         <v>52.12</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1921,7 +1965,7 @@
         <v>52.12</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -1944,7 +1988,7 @@
         <v>184.15</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -1967,7 +2011,7 @@
         <v>52.12</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1990,7 +2034,7 @@
         <v>52.12</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -2013,7 +2057,7 @@
         <v>52.12</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -2036,7 +2080,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
@@ -2059,7 +2103,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
@@ -2082,7 +2126,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
@@ -2105,7 +2149,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -2128,7 +2172,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
@@ -2151,7 +2195,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
@@ -2174,7 +2218,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
@@ -2197,7 +2241,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
@@ -2220,7 +2264,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>29</v>
       </c>
@@ -2243,7 +2287,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
@@ -2266,7 +2310,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>29</v>
       </c>
@@ -2289,7 +2333,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>29</v>
       </c>
@@ -2312,7 +2356,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>29</v>
       </c>
@@ -2335,7 +2379,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -2358,7 +2402,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>29</v>
       </c>
@@ -2381,7 +2425,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>29</v>
       </c>
@@ -2404,7 +2448,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>29</v>
       </c>
@@ -2427,7 +2471,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>29</v>
       </c>
@@ -2450,7 +2494,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>29</v>
       </c>
@@ -2473,7 +2517,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>29</v>
       </c>
@@ -2496,7 +2540,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>29</v>
       </c>
@@ -2519,7 +2563,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>29</v>
       </c>
@@ -2542,7 +2586,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>29</v>
       </c>
@@ -2565,7 +2609,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>29</v>
       </c>
@@ -2588,7 +2632,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>29</v>
       </c>
@@ -2611,7 +2655,7 @@
         <v>38.06</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>29</v>
       </c>
@@ -2634,7 +2678,7 @@
         <v>37.47</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>29</v>
       </c>
@@ -2657,7 +2701,7 @@
         <v>37.47</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>29</v>
       </c>
@@ -2680,7 +2724,7 @@
         <v>37.47</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>29</v>
       </c>
@@ -2703,7 +2747,7 @@
         <v>37.47</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>29</v>
       </c>
@@ -2726,7 +2770,7 @@
         <v>37.47</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>29</v>
       </c>
@@ -2749,7 +2793,7 @@
         <v>37.47</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>29</v>
       </c>
@@ -2772,7 +2816,7 @@
         <v>37.47</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>29</v>
       </c>
@@ -2795,7 +2839,7 @@
         <v>37.47</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>29</v>
       </c>
@@ -2818,7 +2862,7 @@
         <v>37.47</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>29</v>
       </c>
@@ -2841,7 +2885,7 @@
         <v>37.47</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>29</v>
       </c>
@@ -2864,7 +2908,7 @@
         <v>37.47</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>29</v>
       </c>
@@ -2887,7 +2931,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>29</v>
       </c>
@@ -2910,7 +2954,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>29</v>
       </c>
@@ -2933,7 +2977,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>29</v>
       </c>
@@ -2956,7 +3000,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>29</v>
       </c>
@@ -2979,7 +3023,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>29</v>
       </c>
@@ -3002,7 +3046,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>29</v>
       </c>
@@ -3025,7 +3069,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>29</v>
       </c>
@@ -3048,7 +3092,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>29</v>
       </c>
@@ -3071,7 +3115,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>29</v>
       </c>
@@ -3094,7 +3138,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>29</v>
       </c>
@@ -3117,7 +3161,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>29</v>
       </c>
@@ -3140,7 +3184,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>29</v>
       </c>
@@ -3163,7 +3207,7 @@
         <v>11.16</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>29</v>
       </c>
@@ -3186,7 +3230,7 @@
         <v>11.16</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>29</v>
       </c>
@@ -3209,7 +3253,7 @@
         <v>11.16</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>29</v>
       </c>
@@ -3232,7 +3276,7 @@
         <v>15.72</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>29</v>
       </c>
@@ -3255,7 +3299,7 @@
         <v>17.04</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>29</v>
       </c>
@@ -3278,7 +3322,7 @@
         <v>15.72</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>29</v>
       </c>
@@ -3301,7 +3345,7 @@
         <v>15.72</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>29</v>
       </c>
@@ -3324,7 +3368,7 @@
         <v>17.04</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>29</v>
       </c>
@@ -3347,7 +3391,7 @@
         <v>24.68</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>29</v>
       </c>
@@ -3370,7 +3414,7 @@
         <v>24.68</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>29</v>
       </c>
@@ -3393,7 +3437,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>29</v>
       </c>
@@ -3416,7 +3460,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>29</v>
       </c>
@@ -3439,7 +3483,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>29</v>
       </c>
@@ -3462,7 +3506,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>29</v>
       </c>
@@ -3485,7 +3529,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>29</v>
       </c>
@@ -3508,7 +3552,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>29</v>
       </c>
@@ -3531,7 +3575,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>29</v>
       </c>
@@ -3554,7 +3598,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>29</v>
       </c>
@@ -3577,7 +3621,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>29</v>
       </c>
@@ -3600,7 +3644,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>29</v>
       </c>
@@ -3623,7 +3667,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>29</v>
       </c>
@@ -3646,7 +3690,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>29</v>
       </c>
@@ -3669,7 +3713,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>29</v>
       </c>
@@ -3692,7 +3736,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>29</v>
       </c>
@@ -3715,7 +3759,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>29</v>
       </c>
@@ -3738,7 +3782,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>29</v>
       </c>
@@ -3761,7 +3805,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>29</v>
       </c>
@@ -3784,7 +3828,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>29</v>
       </c>
@@ -3807,7 +3851,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>29</v>
       </c>
@@ -3830,7 +3874,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>29</v>
       </c>
@@ -3853,7 +3897,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>29</v>
       </c>
@@ -3876,7 +3920,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>29</v>
       </c>
@@ -3899,7 +3943,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>29</v>
       </c>
@@ -3922,7 +3966,7 @@
         <v>34.08</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>29</v>
       </c>
@@ -3945,7 +3989,7 @@
         <v>32.909999999999997</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>29</v>
       </c>
@@ -3968,7 +4012,7 @@
         <v>32.909999999999997</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>29</v>
       </c>
@@ -3991,7 +4035,7 @@
         <v>32.909999999999997</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>29</v>
       </c>
@@ -4014,7 +4058,7 @@
         <v>32.909999999999997</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>29</v>
       </c>
@@ -4037,7 +4081,7 @@
         <v>32.909999999999997</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>29</v>
       </c>
@@ -4060,7 +4104,7 @@
         <v>32.909999999999997</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>29</v>
       </c>
@@ -4083,7 +4127,7 @@
         <v>32.909999999999997</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>29</v>
       </c>
@@ -4106,7 +4150,7 @@
         <v>32.909999999999997</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>29</v>
       </c>
@@ -4129,7 +4173,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>29</v>
       </c>
@@ -4152,7 +4196,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>29</v>
       </c>
@@ -4175,7 +4219,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>29</v>
       </c>
@@ -4198,7 +4242,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>29</v>
       </c>
@@ -4221,7 +4265,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>29</v>
       </c>
@@ -4244,7 +4288,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>29</v>
       </c>
@@ -4267,7 +4311,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>29</v>
       </c>
@@ -4290,7 +4334,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="131" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="131" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>29</v>
       </c>
@@ -4313,7 +4357,7 @@
         <v>58.765000000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="132" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>29</v>
       </c>
@@ -4336,7 +4380,7 @@
         <v>58.765000000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="133" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>29</v>
       </c>
@@ -4359,7 +4403,7 @@
         <v>67.573999999999998</v>
       </c>
     </row>
-    <row r="134" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="134" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>29</v>
       </c>
@@ -4382,7 +4426,7 @@
         <v>67.573999999999998</v>
       </c>
     </row>
-    <row r="135" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="135" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>29</v>
       </c>
@@ -4405,7 +4449,7 @@
         <v>67.573999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="136" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>29</v>
       </c>
@@ -4428,7 +4472,7 @@
         <v>67.573999999999998</v>
       </c>
     </row>
-    <row r="137" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="137" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>29</v>
       </c>
@@ -4451,7 +4495,7 @@
         <v>67.573999999999998</v>
       </c>
     </row>
-    <row r="138" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="138" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>29</v>
       </c>
@@ -4474,7 +4518,7 @@
         <v>67.573999999999998</v>
       </c>
     </row>
-    <row r="139" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="139" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>29</v>
       </c>
@@ -4497,7 +4541,7 @@
         <v>67.573999999999998</v>
       </c>
     </row>
-    <row r="140" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="140" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>29</v>
       </c>
@@ -4520,12 +4564,12 @@
         <v>67.573999999999998</v>
       </c>
     </row>
-    <row r="141" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="141" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>274</v>
@@ -4543,7 +4587,7 @@
         <v>73.462000000000003</v>
       </c>
     </row>
-    <row r="142" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="142" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>29</v>
       </c>
@@ -4566,7 +4610,7 @@
         <v>73.462000000000003</v>
       </c>
     </row>
-    <row r="143" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="143" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>29</v>
       </c>
@@ -4589,7 +4633,7 @@
         <v>73.462000000000003</v>
       </c>
     </row>
-    <row r="144" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="144" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>29</v>
       </c>
@@ -4612,12 +4656,12 @@
         <v>73.462000000000003</v>
       </c>
     </row>
-    <row r="145" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="145" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>280</v>
@@ -4637,16 +4681,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C9">
-    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C130">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C31">
-    <cfRule type="duplicateValues" dxfId="1" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C131:C145">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>